<commit_message>
add repo jitpack add testng
</commit_message>
<xml_diff>
--- a/LogDolar.xlsx
+++ b/LogDolar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="35">
   <si>
     <t xml:space="preserve">Dia Actualización Valor Dólar</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t xml:space="preserve">01/01/2023 12:25</t>
+  </si>
+  <si>
+    <t>30/12</t>
+  </si>
+  <si>
+    <t>Mercado cerrado</t>
+  </si>
+  <si>
+    <t>01/01/2023 02:59</t>
+  </si>
+  <si>
+    <t>848,25</t>
   </si>
 </sst>
 </file>
@@ -236,7 +248,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
@@ -244,10 +256,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="28.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="8.72"/>
+    <col min="1" max="2" customWidth="true" hidden="false" style="1" width="28.37" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="17.55" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="2" width="15.18" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="1024" customWidth="false" hidden="false" style="1" width="8.72" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,6 +778,20 @@
       </c>
       <c r="D37" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Directory driver, xlsx
</commit_message>
<xml_diff>
--- a/LogDolar.xlsx
+++ b/LogDolar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="36">
   <si>
     <t xml:space="preserve">Dia Actualización Valor Dólar</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>848,25</t>
+  </si>
+  <si>
+    <t>01/01/2023 03:40</t>
   </si>
 </sst>
 </file>
@@ -248,7 +251,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
@@ -794,6 +797,20 @@
         <v>34</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update ChromeDriver update LogDolar.xlsx Browser Changes. Now use Chrome Delete .zip and logExcel
</commit_message>
<xml_diff>
--- a/LogDolar.xlsx
+++ b/LogDolar.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">Dia Actualización Valor Dólar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">Dia- Hora Ultima Actualizacion </t>
   </si>
   <si>
     <t xml:space="preserve">EstadoMercado</t>
@@ -115,19 +115,40 @@
     <t xml:space="preserve">01/01/2023 12:25</t>
   </si>
   <si>
-    <t>30/12</t>
-  </si>
-  <si>
-    <t>Mercado cerrado</t>
-  </si>
-  <si>
-    <t>01/01/2023 02:59</t>
+    <t xml:space="preserve">01/01/2023 02:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2023 03:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info en tiempo real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2023 04:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2023 04:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2023 04:54</t>
+  </si>
+  <si>
+    <t>23:00:03</t>
+  </si>
+  <si>
+    <t>Info en tiempo real</t>
+  </si>
+  <si>
+    <t>02/01/2023 05:14</t>
   </si>
   <si>
     <t>848,25</t>
   </si>
   <si>
-    <t>01/01/2023 03:40</t>
+    <t>02/01/2023 05:16</t>
   </si>
 </sst>
 </file>
@@ -251,17 +272,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" customWidth="true" hidden="false" style="1" width="28.37" collapsed="false" outlineLevel="0"/>
+    <col min="1" max="2" customWidth="true" hidden="false" style="1" width="28.36" collapsed="false" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="1" width="17.55" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="2" width="15.18" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="2" width="15.17" collapsed="false" outlineLevel="0"/>
     <col min="5" max="1024" customWidth="false" hidden="false" style="1" width="8.72" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
@@ -783,37 +804,107 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="s">
+    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D38" t="s">
+      <c r="B40" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="C40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>